<commit_message>
cambios en el exel
</commit_message>
<xml_diff>
--- a/estructurasDatosWordix.xlsx
+++ b/estructurasDatosWordix.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710B0E66-1967-4AAB-A013-7A45D760B946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraDatos" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>$coleccionPalabras=</t>
   </si>
@@ -62,13 +63,16 @@
   </si>
   <si>
     <t>¿Para qué se utiliza?: guarda las palabras que se pueden elegidas para jugar wordix</t>
+  </si>
+  <si>
+    <t>asdasdas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,14 +163,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -176,13 +180,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -220,7 +232,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -254,6 +266,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -288,9 +301,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -463,14 +477,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -481,12 +495,12 @@
     <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -512,7 +526,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -535,32 +549,37 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Agregue celdas al excel (colecccionPalabras)
</commit_message>
<xml_diff>
--- a/estructurasDatosWordix.xlsx
+++ b/estructurasDatosWordix.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710B0E66-1967-4AAB-A013-7A45D760B946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14AAF60-2104-4B75-A340-9574FB70F71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22695" yWindow="1725" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraDatos" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>$coleccionPalabras=</t>
   </si>
@@ -53,9 +53,6 @@
     <t>//valores</t>
   </si>
   <si>
-    <t>**** COMPLETAR ****</t>
-  </si>
-  <si>
     <t>Ejemplo de cómo representar las estructuras de datos según lo visto en teoría:</t>
   </si>
   <si>
@@ -65,14 +62,56 @@
     <t>¿Para qué se utiliza?: guarda las palabras que se pueden elegidas para jugar wordix</t>
   </si>
   <si>
-    <t>asdasdas</t>
+    <t xml:space="preserve">QUESO </t>
+  </si>
+  <si>
+    <t>GOTAS</t>
+  </si>
+  <si>
+    <t>HUEVO</t>
+  </si>
+  <si>
+    <t>TINTO</t>
+  </si>
+  <si>
+    <t>NAVES</t>
+  </si>
+  <si>
+    <t>VERDE</t>
+  </si>
+  <si>
+    <t>MELON</t>
+  </si>
+  <si>
+    <t>YUYOS</t>
+  </si>
+  <si>
+    <t>PIANO</t>
+  </si>
+  <si>
+    <t>SILLA</t>
+  </si>
+  <si>
+    <t>LAPIZ</t>
+  </si>
+  <si>
+    <t>BRUMA</t>
+  </si>
+  <si>
+    <t>RATON</t>
+  </si>
+  <si>
+    <t>PISOS</t>
+  </si>
+  <si>
+    <t>CABLE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +146,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -158,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -174,6 +221,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -192,9 +248,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -232,9 +288,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -267,9 +323,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -302,9 +375,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -478,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,12 +585,12 @@
     <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -526,7 +616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -549,39 +639,163 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="8">
+        <v>0</v>
+      </c>
+      <c r="C13" s="8">
+        <v>1</v>
+      </c>
+      <c r="D13" s="8">
+        <v>2</v>
+      </c>
+      <c r="E13" s="8">
+        <v>3</v>
+      </c>
+      <c r="F13" s="8">
+        <v>4</v>
+      </c>
+      <c r="G13" s="8">
+        <v>5</v>
+      </c>
+      <c r="H13" s="8">
+        <v>6</v>
+      </c>
+      <c r="I13" s="8">
+        <v>7</v>
+      </c>
+      <c r="J13" s="8">
+        <v>8</v>
+      </c>
+      <c r="K13" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="D14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="8">
+        <v>10</v>
+      </c>
+      <c r="C15" s="8">
+        <v>11</v>
+      </c>
+      <c r="D15" s="8">
+        <v>12</v>
+      </c>
+      <c r="E15" s="8">
+        <v>13</v>
+      </c>
+      <c r="F15" s="8">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
+      <c r="G15" s="8">
+        <v>15</v>
+      </c>
+      <c r="H15" s="8">
+        <v>16</v>
+      </c>
+      <c r="I15" s="8">
+        <v>17</v>
+      </c>
+      <c r="J15" s="8">
+        <v>18</v>
+      </c>
+      <c r="K15" s="8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregue Arreglos al excel (fijarse cuales faltan)
</commit_message>
<xml_diff>
--- a/estructurasDatosWordix.xlsx
+++ b/estructurasDatosWordix.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14AAF60-2104-4B75-A340-9574FB70F71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BD373F-E079-40AD-9C2E-6C732EDAAEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22695" yWindow="1725" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraDatos" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="124">
   <si>
     <t>$coleccionPalabras=</t>
   </si>
@@ -105,13 +105,308 @@
   </si>
   <si>
     <t>CABLE</t>
+  </si>
+  <si>
+    <t>Tipo: Indexado</t>
+  </si>
+  <si>
+    <t>Tipos de datos:String</t>
+  </si>
+  <si>
+    <t>$teclado=</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V </t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>Tipo: Asociativo</t>
+  </si>
+  <si>
+    <t>tipo de datos: String</t>
+  </si>
+  <si>
+    <t>Se utiliza para: guarda las palabras que se pueden elegidas para jugar wordix</t>
+  </si>
+  <si>
+    <t>Se utiliza para: Ver el estado de una letra</t>
+  </si>
+  <si>
+    <t>$ordenTeclado=</t>
+  </si>
+  <si>
+    <t>salto</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Tipo de datos: String</t>
+  </si>
+  <si>
+    <t>Se utiliza para: Mostrar el orden en que aparecen las letras por consola (simula un teclado), salto refiere a un \n</t>
+  </si>
+  <si>
+    <t>$estructuraPalabraIntento=</t>
+  </si>
+  <si>
+    <t>$puntajeLetras=</t>
+  </si>
+  <si>
+    <t>"A"</t>
+  </si>
+  <si>
+    <t>"E"</t>
+  </si>
+  <si>
+    <r>
+      <t>"I</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>"O"</t>
+  </si>
+  <si>
+    <t>"U"</t>
+  </si>
+  <si>
+    <t>"B"</t>
+  </si>
+  <si>
+    <t>"C"</t>
+  </si>
+  <si>
+    <t>"D"</t>
+  </si>
+  <si>
+    <t>"F"</t>
+  </si>
+  <si>
+    <t>"G"</t>
+  </si>
+  <si>
+    <t>"H"</t>
+  </si>
+  <si>
+    <t>"J"</t>
+  </si>
+  <si>
+    <t>"K"</t>
+  </si>
+  <si>
+    <t>"L"</t>
+  </si>
+  <si>
+    <t>"M"</t>
+  </si>
+  <si>
+    <t>"N"</t>
+  </si>
+  <si>
+    <t>"Ñ"</t>
+  </si>
+  <si>
+    <t>"P"</t>
+  </si>
+  <si>
+    <t>"Q"</t>
+  </si>
+  <si>
+    <t>"S"</t>
+  </si>
+  <si>
+    <t>"T"</t>
+  </si>
+  <si>
+    <t>"V"</t>
+  </si>
+  <si>
+    <t>"W"</t>
+  </si>
+  <si>
+    <t>"X"</t>
+  </si>
+  <si>
+    <t>"Y"</t>
+  </si>
+  <si>
+    <t>"Z"</t>
+  </si>
+  <si>
+    <t>Tipo de datos:Entero</t>
+  </si>
+  <si>
+    <t>Se utiliza para: Asignarle un valor a cada letra del abecedario</t>
+  </si>
+  <si>
+    <t>$partida=</t>
+  </si>
+  <si>
+    <t>$palabraWordix</t>
+  </si>
+  <si>
+    <t>$nombreUsuario</t>
+  </si>
+  <si>
+    <t>$puntaje</t>
+  </si>
+  <si>
+    <t>$nroIntento</t>
+  </si>
+  <si>
+    <t>"PalabraWordix"</t>
+  </si>
+  <si>
+    <t>"jugador"</t>
+  </si>
+  <si>
+    <t>"intentos"</t>
+  </si>
+  <si>
+    <t>"puntaje"</t>
+  </si>
+  <si>
+    <t>Tipo:Asociativo</t>
+  </si>
+  <si>
+    <t>Tipo de datos: String y Enteros</t>
+  </si>
+  <si>
+    <t>Se utiliza para: Guardar los valores, el string de la palabra, el string del nombre del jugador, el entero de la cantidad de intentos y el entero del puntaje obtenido</t>
+  </si>
+  <si>
+    <t>$ejemploPartidas=</t>
+  </si>
+  <si>
+    <t>"palabraWordix"</t>
+  </si>
+  <si>
+    <t>Emilia</t>
+  </si>
+  <si>
+    <t>Adriano</t>
+  </si>
+  <si>
+    <t>Facu</t>
+  </si>
+  <si>
+    <t>Eva</t>
+  </si>
+  <si>
+    <t>Tomi</t>
+  </si>
+  <si>
+    <t>Agus</t>
+  </si>
+  <si>
+    <t>Ludmi</t>
+  </si>
+  <si>
+    <t>Cristian</t>
+  </si>
+  <si>
+    <t>ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>Tipo:Multidimensional</t>
+  </si>
+  <si>
+    <t>Tipo de datos:String y Enteros</t>
+  </si>
+  <si>
+    <t>Se utiliza para: Guardar los ejemplos de partidas ya completadas.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +453,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -167,7 +468,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -201,11 +502,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -225,6 +555,32 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -568,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,34 +1059,34 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="9" t="s">
+      <c r="J14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="K14" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -767,35 +1123,1125 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="9" t="s">
+      <c r="J16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K16" s="9" t="s">
+      <c r="K16" s="1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2">
+        <v>2</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3</v>
+      </c>
+      <c r="F22" s="2">
+        <v>4</v>
+      </c>
+      <c r="G22" s="2">
+        <v>5</v>
+      </c>
+      <c r="H22" s="2">
+        <v>6</v>
+      </c>
+      <c r="I22" s="2">
+        <v>7</v>
+      </c>
+      <c r="J22" s="2">
+        <v>8</v>
+      </c>
+      <c r="K22" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="I23" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="J23" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="K23" s="19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="2">
+        <v>10</v>
+      </c>
+      <c r="C25" s="2">
+        <v>11</v>
+      </c>
+      <c r="D25" s="2">
+        <v>12</v>
+      </c>
+      <c r="E25" s="2">
+        <v>13</v>
+      </c>
+      <c r="F25" s="2">
+        <v>14</v>
+      </c>
+      <c r="G25" s="2">
+        <v>15</v>
+      </c>
+      <c r="H25" s="2">
+        <v>16</v>
+      </c>
+      <c r="I25" s="2">
+        <v>17</v>
+      </c>
+      <c r="J25" s="2">
+        <v>18</v>
+      </c>
+      <c r="K25" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="G26" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="H26" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="I26" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="J26" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="K26" s="19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <v>20</v>
+      </c>
+      <c r="C28" s="2">
+        <v>21</v>
+      </c>
+      <c r="D28" s="2">
+        <v>22</v>
+      </c>
+      <c r="E28" s="2">
+        <v>23</v>
+      </c>
+      <c r="F28" s="2">
+        <v>24</v>
+      </c>
+      <c r="G28" s="2">
+        <v>25</v>
+      </c>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="G29" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0</v>
+      </c>
+      <c r="C35" s="2">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2">
+        <v>2</v>
+      </c>
+      <c r="E35" s="2">
+        <v>3</v>
+      </c>
+      <c r="F35" s="2">
+        <v>4</v>
+      </c>
+      <c r="G35" s="2">
+        <v>5</v>
+      </c>
+      <c r="H35" s="2">
+        <v>6</v>
+      </c>
+      <c r="I35" s="2">
+        <v>7</v>
+      </c>
+      <c r="J35" s="2">
+        <v>8</v>
+      </c>
+      <c r="K35" s="2">
+        <v>9</v>
+      </c>
+      <c r="L35" s="2">
+        <v>10</v>
+      </c>
+      <c r="M35" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>12</v>
+      </c>
+      <c r="C37" s="2">
+        <v>13</v>
+      </c>
+      <c r="D37" s="2">
+        <v>14</v>
+      </c>
+      <c r="E37" s="2">
+        <v>15</v>
+      </c>
+      <c r="F37" s="2">
+        <v>16</v>
+      </c>
+      <c r="G37" s="2">
+        <v>17</v>
+      </c>
+      <c r="H37" s="2">
+        <v>18</v>
+      </c>
+      <c r="I37" s="2">
+        <v>19</v>
+      </c>
+      <c r="J37" s="2">
+        <v>20</v>
+      </c>
+      <c r="K37" s="2">
+        <v>21</v>
+      </c>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B39" s="2">
+        <v>22</v>
+      </c>
+      <c r="C39" s="2">
+        <v>23</v>
+      </c>
+      <c r="D39" s="2">
+        <v>24</v>
+      </c>
+      <c r="E39" s="2">
+        <v>25</v>
+      </c>
+      <c r="F39" s="2">
+        <v>26</v>
+      </c>
+      <c r="G39" s="2">
+        <v>27</v>
+      </c>
+      <c r="H39" s="2">
+        <v>28</v>
+      </c>
+      <c r="I39" s="2">
+        <v>29</v>
+      </c>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B41" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B43" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B44" s="11"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B48" s="2">
+        <v>0</v>
+      </c>
+      <c r="C48" s="2">
+        <v>1</v>
+      </c>
+      <c r="D48" s="2">
+        <v>2</v>
+      </c>
+      <c r="E48" s="2">
+        <v>3</v>
+      </c>
+      <c r="F48" s="2">
+        <v>4</v>
+      </c>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B49" s="1">
+        <v>1</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1">
+        <v>1</v>
+      </c>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="12"/>
+      <c r="K49" s="12"/>
+      <c r="L49" s="12"/>
+      <c r="M49" s="12"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" s="15"/>
+      <c r="B50" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G50" s="13"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+      <c r="K50" s="12"/>
+      <c r="L50" s="12"/>
+      <c r="M50" s="12"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B51" s="2">
+        <v>5</v>
+      </c>
+      <c r="C51" s="2">
+        <v>6</v>
+      </c>
+      <c r="D51" s="2">
+        <v>7</v>
+      </c>
+      <c r="E51" s="2">
+        <v>8</v>
+      </c>
+      <c r="F51" s="2">
+        <v>9</v>
+      </c>
+      <c r="G51" s="2">
+        <v>10</v>
+      </c>
+      <c r="H51" s="2">
+        <v>11</v>
+      </c>
+      <c r="I51" s="2">
+        <v>12</v>
+      </c>
+      <c r="J51" s="2">
+        <v>13</v>
+      </c>
+      <c r="K51" s="2">
+        <v>14</v>
+      </c>
+      <c r="L51" s="12"/>
+      <c r="M51" s="12"/>
+      <c r="N51" s="11"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" s="11"/>
+      <c r="B52" s="1">
+        <v>2</v>
+      </c>
+      <c r="C52" s="1">
+        <v>2</v>
+      </c>
+      <c r="D52" s="1">
+        <v>2</v>
+      </c>
+      <c r="E52" s="1">
+        <v>2</v>
+      </c>
+      <c r="F52" s="1">
+        <v>2</v>
+      </c>
+      <c r="G52" s="1">
+        <v>2</v>
+      </c>
+      <c r="H52" s="1">
+        <v>2</v>
+      </c>
+      <c r="I52" s="1">
+        <v>2</v>
+      </c>
+      <c r="J52" s="1">
+        <v>2</v>
+      </c>
+      <c r="K52" s="1">
+        <v>2</v>
+      </c>
+      <c r="L52" s="12"/>
+      <c r="M52" s="12"/>
+      <c r="N52" s="11"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L53" s="13"/>
+      <c r="M53" s="12"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" s="11"/>
+      <c r="B54" s="14">
+        <v>15</v>
+      </c>
+      <c r="C54" s="14">
+        <v>16</v>
+      </c>
+      <c r="D54" s="14">
+        <v>17</v>
+      </c>
+      <c r="E54" s="14">
+        <v>18</v>
+      </c>
+      <c r="F54" s="14">
+        <v>19</v>
+      </c>
+      <c r="G54" s="14">
+        <v>20</v>
+      </c>
+      <c r="H54" s="14">
+        <v>21</v>
+      </c>
+      <c r="I54" s="14">
+        <v>22</v>
+      </c>
+      <c r="J54" s="14">
+        <v>23</v>
+      </c>
+      <c r="K54" s="14">
+        <v>24</v>
+      </c>
+      <c r="L54" s="9">
+        <v>25</v>
+      </c>
+      <c r="M54" s="9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B55" s="1">
+        <v>3</v>
+      </c>
+      <c r="C55" s="1">
+        <v>3</v>
+      </c>
+      <c r="D55" s="1">
+        <v>3</v>
+      </c>
+      <c r="E55" s="1">
+        <v>3</v>
+      </c>
+      <c r="F55" s="1">
+        <v>3</v>
+      </c>
+      <c r="G55" s="1">
+        <v>3</v>
+      </c>
+      <c r="H55" s="1">
+        <v>3</v>
+      </c>
+      <c r="I55" s="1">
+        <v>3</v>
+      </c>
+      <c r="J55" s="1">
+        <v>3</v>
+      </c>
+      <c r="K55" s="1">
+        <v>3</v>
+      </c>
+      <c r="L55" s="1">
+        <v>3</v>
+      </c>
+      <c r="M55" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B57" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B58" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B59" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>98</v>
+      </c>
+      <c r="B61" s="2">
+        <v>0</v>
+      </c>
+      <c r="C61" s="2">
+        <v>1</v>
+      </c>
+      <c r="D61" s="2">
+        <v>2</v>
+      </c>
+      <c r="E61" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B62" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B63" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>110</v>
+      </c>
+      <c r="B68" s="2">
+        <v>0</v>
+      </c>
+      <c r="C68" s="2">
+        <v>1</v>
+      </c>
+      <c r="D68" s="2">
+        <v>2</v>
+      </c>
+      <c r="E68" s="2">
+        <v>3</v>
+      </c>
+      <c r="F68" s="2">
+        <v>4</v>
+      </c>
+      <c r="G68" s="2">
+        <v>5</v>
+      </c>
+      <c r="H68" s="2">
+        <v>6</v>
+      </c>
+      <c r="I68" s="2">
+        <v>7</v>
+      </c>
+      <c r="J68" s="2">
+        <v>8</v>
+      </c>
+      <c r="K68" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>111</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>104</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>105</v>
+      </c>
+      <c r="B71" s="1">
+        <v>0</v>
+      </c>
+      <c r="C71" s="1">
+        <v>3</v>
+      </c>
+      <c r="D71" s="1">
+        <v>2</v>
+      </c>
+      <c r="E71" s="1">
+        <v>2</v>
+      </c>
+      <c r="F71" s="1">
+        <v>5</v>
+      </c>
+      <c r="G71" s="1">
+        <v>1</v>
+      </c>
+      <c r="H71" s="1">
+        <v>4</v>
+      </c>
+      <c r="I71" s="1">
+        <v>5</v>
+      </c>
+      <c r="J71" s="1">
+        <v>4</v>
+      </c>
+      <c r="K71" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>106</v>
+      </c>
+      <c r="B72" s="1">
+        <v>0</v>
+      </c>
+      <c r="C72" s="1">
+        <v>14</v>
+      </c>
+      <c r="D72" s="1">
+        <v>13</v>
+      </c>
+      <c r="E72" s="1">
+        <v>15</v>
+      </c>
+      <c r="F72" s="1">
+        <v>12</v>
+      </c>
+      <c r="G72" s="1">
+        <v>15</v>
+      </c>
+      <c r="H72" s="1">
+        <v>13</v>
+      </c>
+      <c r="I72" s="1">
+        <v>11</v>
+      </c>
+      <c r="J72" s="1">
+        <v>14</v>
+      </c>
+      <c r="K72" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B73" s="16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B74" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B75" s="17" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregue Arreglos al excel, fijarse cuales faltan
</commit_message>
<xml_diff>
--- a/estructurasDatosWordix.xlsx
+++ b/estructurasDatosWordix.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BD373F-E079-40AD-9C2E-6C732EDAAEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A61216-8154-4CBE-A1D9-BDA27F408732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -535,7 +535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -557,14 +557,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -576,15 +569,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -924,9 +908,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N75"/>
+  <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
       <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
@@ -1205,34 +1189,34 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="G23" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="H23" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="I23" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="J23" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="K23" s="19" t="s">
+      <c r="B23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1301,34 +1285,34 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="G26" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="H26" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="I26" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="J26" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="K26" s="19" t="s">
+      <c r="B26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K26" s="1" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1389,22 +1373,22 @@
       <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="F29" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="G29" s="19" t="s">
+      <c r="B29" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>120</v>
       </c>
       <c r="H29" s="7"/>
@@ -1437,7 +1421,7 @@
       <c r="K30" s="7"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1659,7 +1643,7 @@
       <c r="M40" s="7"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="9" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1669,12 +1653,9 @@
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="11" t="s">
+      <c r="B43" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="11"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -1710,7 +1691,7 @@
       <c r="L48" s="7"/>
       <c r="M48" s="7"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B49" s="1">
         <v>1</v>
       </c>
@@ -1726,16 +1707,16 @@
       <c r="F49" s="1">
         <v>1</v>
       </c>
-      <c r="G49" s="12"/>
-      <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
-      <c r="J49" s="12"/>
-      <c r="K49" s="12"/>
-      <c r="L49" s="12"/>
-      <c r="M49" s="12"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="15"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="7"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="12"/>
       <c r="B50" s="1" t="s">
         <v>70</v>
       </c>
@@ -1751,15 +1732,15 @@
       <c r="F50" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G50" s="13"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
-      <c r="J50" s="12"/>
-      <c r="K50" s="12"/>
-      <c r="L50" s="12"/>
-      <c r="M50" s="12"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G50" s="10"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B51" s="2">
         <v>5</v>
       </c>
@@ -1790,12 +1771,10 @@
       <c r="K51" s="2">
         <v>14</v>
       </c>
-      <c r="L51" s="12"/>
-      <c r="M51" s="12"/>
-      <c r="N51" s="11"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="11"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="7"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B52" s="1">
         <v>2</v>
       </c>
@@ -1826,11 +1805,10 @@
       <c r="K52" s="1">
         <v>2</v>
       </c>
-      <c r="L52" s="12"/>
-      <c r="M52" s="12"/>
-      <c r="N52" s="11"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L52" s="7"/>
+      <c r="M52" s="7"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>75</v>
       </c>
@@ -1861,49 +1839,48 @@
       <c r="K53" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="L53" s="13"/>
-      <c r="M53" s="12"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="11"/>
-      <c r="B54" s="14">
+      <c r="L53" s="10"/>
+      <c r="M53" s="7"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B54" s="11">
         <v>15</v>
       </c>
-      <c r="C54" s="14">
+      <c r="C54" s="11">
         <v>16</v>
       </c>
-      <c r="D54" s="14">
+      <c r="D54" s="11">
         <v>17</v>
       </c>
-      <c r="E54" s="14">
+      <c r="E54" s="11">
         <v>18</v>
       </c>
-      <c r="F54" s="14">
+      <c r="F54" s="11">
         <v>19</v>
       </c>
-      <c r="G54" s="14">
+      <c r="G54" s="11">
         <v>20</v>
       </c>
-      <c r="H54" s="14">
+      <c r="H54" s="11">
         <v>21</v>
       </c>
-      <c r="I54" s="14">
+      <c r="I54" s="11">
         <v>22</v>
       </c>
-      <c r="J54" s="14">
+      <c r="J54" s="11">
         <v>23</v>
       </c>
-      <c r="K54" s="14">
+      <c r="K54" s="11">
         <v>24</v>
       </c>
-      <c r="L54" s="9">
+      <c r="L54" s="2">
         <v>25</v>
       </c>
-      <c r="M54" s="9">
+      <c r="M54" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B55" s="1">
         <v>3</v>
       </c>
@@ -1941,7 +1918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
         <v>85</v>
       </c>
@@ -1979,22 +1956,22 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B57" s="16" t="s">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B57" s="13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B58" s="17" t="s">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B58" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B59" s="17" t="s">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B59" s="13" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>98</v>
       </c>
@@ -2011,8 +1988,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B62" s="18" t="s">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C62" s="1" t="s">
@@ -2025,8 +2002,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B63" s="18" t="s">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
         <v>103</v>
       </c>
       <c r="C63" s="1" t="s">
@@ -2039,7 +2016,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>107</v>
       </c>
@@ -2230,17 +2207,17 @@
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B73" s="16" t="s">
+      <c r="B73" s="13" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B74" s="17" t="s">
+      <c r="B74" s="13" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B75" s="17" t="s">
+      <c r="B75" s="13" t="s">
         <v>123</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Terminado el excel, arreglar caso 5
</commit_message>
<xml_diff>
--- a/estructurasDatosWordix.xlsx
+++ b/estructurasDatosWordix.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A61216-8154-4CBE-A1D9-BDA27F408732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B45CCD-7856-4A39-8A55-90FA5B5168F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraDatos" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="135">
   <si>
     <t>$coleccionPalabras=</t>
   </si>
@@ -219,9 +219,6 @@
   </si>
   <si>
     <t>Se utiliza para: Mostrar el orden en que aparecen las letras por consola (simula un teclado), salto refiere a un \n</t>
-  </si>
-  <si>
-    <t>$estructuraPalabraIntento=</t>
   </si>
   <si>
     <t>$puntajeLetras=</t>
@@ -401,12 +398,48 @@
   <si>
     <t>Se utiliza para: Guardar los ejemplos de partidas ya completadas.</t>
   </si>
+  <si>
+    <t>$resumenJugador=</t>
+  </si>
+  <si>
+    <t>"cantPartidas"</t>
+  </si>
+  <si>
+    <t>"totalPuntaje"</t>
+  </si>
+  <si>
+    <t>"victorias"</t>
+  </si>
+  <si>
+    <t>"porcentajeVictorias"</t>
+  </si>
+  <si>
+    <t>"int1"</t>
+  </si>
+  <si>
+    <t>"int2"</t>
+  </si>
+  <si>
+    <t>"int3"</t>
+  </si>
+  <si>
+    <t>"Int4"</t>
+  </si>
+  <si>
+    <t>"int5"</t>
+  </si>
+  <si>
+    <t>"int6"</t>
+  </si>
+  <si>
+    <t>$jugadorNombre</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -455,6 +488,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -535,7 +576,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -570,6 +611,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -908,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M75"/>
+  <dimension ref="A1:O78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,34 +1232,34 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1286,34 +1328,34 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1374,22 +1416,22 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -1657,31 +1699,50 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>69</v>
-      </c>
+      <c r="B47" s="2">
+        <v>0</v>
+      </c>
+      <c r="C47" s="2">
+        <v>1</v>
+      </c>
+      <c r="D47" s="2">
+        <v>2</v>
+      </c>
+      <c r="E47" s="2">
+        <v>3</v>
+      </c>
+      <c r="F47" s="2">
+        <v>4</v>
+      </c>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="2">
-        <v>0</v>
-      </c>
-      <c r="C48" s="2">
+      <c r="B48" s="1">
         <v>1</v>
       </c>
-      <c r="D48" s="2">
-        <v>2</v>
-      </c>
-      <c r="E48" s="2">
-        <v>3</v>
-      </c>
-      <c r="F48" s="2">
-        <v>4</v>
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1</v>
+      </c>
+      <c r="F48" s="1">
+        <v>1</v>
       </c>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
@@ -1692,22 +1753,23 @@
       <c r="M48" s="7"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B49" s="1">
-        <v>1</v>
-      </c>
-      <c r="C49" s="1">
-        <v>1</v>
-      </c>
-      <c r="D49" s="1">
-        <v>1</v>
-      </c>
-      <c r="E49" s="1">
-        <v>1</v>
-      </c>
-      <c r="F49" s="1">
-        <v>1</v>
-      </c>
-      <c r="G49" s="7"/>
+      <c r="A49" s="12"/>
+      <c r="B49" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G49" s="10"/>
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
       <c r="J49" s="7"/>
@@ -1716,249 +1778,229 @@
       <c r="M49" s="7"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="12"/>
-      <c r="B50" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G50" s="10"/>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="7"/>
-      <c r="K50" s="7"/>
+      <c r="B50" s="2">
+        <v>5</v>
+      </c>
+      <c r="C50" s="2">
+        <v>6</v>
+      </c>
+      <c r="D50" s="2">
+        <v>7</v>
+      </c>
+      <c r="E50" s="2">
+        <v>8</v>
+      </c>
+      <c r="F50" s="2">
+        <v>9</v>
+      </c>
+      <c r="G50" s="2">
+        <v>10</v>
+      </c>
+      <c r="H50" s="2">
+        <v>11</v>
+      </c>
+      <c r="I50" s="2">
+        <v>12</v>
+      </c>
+      <c r="J50" s="2">
+        <v>13</v>
+      </c>
+      <c r="K50" s="2">
+        <v>14</v>
+      </c>
       <c r="L50" s="7"/>
       <c r="M50" s="7"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B51" s="2">
-        <v>5</v>
-      </c>
-      <c r="C51" s="2">
-        <v>6</v>
-      </c>
-      <c r="D51" s="2">
-        <v>7</v>
-      </c>
-      <c r="E51" s="2">
-        <v>8</v>
-      </c>
-      <c r="F51" s="2">
-        <v>9</v>
-      </c>
-      <c r="G51" s="2">
-        <v>10</v>
-      </c>
-      <c r="H51" s="2">
-        <v>11</v>
-      </c>
-      <c r="I51" s="2">
-        <v>12</v>
-      </c>
-      <c r="J51" s="2">
-        <v>13</v>
-      </c>
-      <c r="K51" s="2">
-        <v>14</v>
+      <c r="B51" s="1">
+        <v>2</v>
+      </c>
+      <c r="C51" s="1">
+        <v>2</v>
+      </c>
+      <c r="D51" s="1">
+        <v>2</v>
+      </c>
+      <c r="E51" s="1">
+        <v>2</v>
+      </c>
+      <c r="F51" s="1">
+        <v>2</v>
+      </c>
+      <c r="G51" s="1">
+        <v>2</v>
+      </c>
+      <c r="H51" s="1">
+        <v>2</v>
+      </c>
+      <c r="I51" s="1">
+        <v>2</v>
+      </c>
+      <c r="J51" s="1">
+        <v>2</v>
+      </c>
+      <c r="K51" s="1">
+        <v>2</v>
       </c>
       <c r="L51" s="7"/>
       <c r="M51" s="7"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B52" s="1">
-        <v>2</v>
-      </c>
-      <c r="C52" s="1">
-        <v>2</v>
-      </c>
-      <c r="D52" s="1">
-        <v>2</v>
-      </c>
-      <c r="E52" s="1">
-        <v>2</v>
-      </c>
-      <c r="F52" s="1">
-        <v>2</v>
-      </c>
-      <c r="G52" s="1">
-        <v>2</v>
-      </c>
-      <c r="H52" s="1">
-        <v>2</v>
-      </c>
-      <c r="I52" s="1">
-        <v>2</v>
-      </c>
-      <c r="J52" s="1">
-        <v>2</v>
-      </c>
-      <c r="K52" s="1">
-        <v>2</v>
-      </c>
-      <c r="L52" s="7"/>
+      <c r="B52" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L52" s="10"/>
       <c r="M52" s="7"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J53" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="K53" s="1" t="s">
+      <c r="B53" s="11">
+        <v>15</v>
+      </c>
+      <c r="C53" s="11">
+        <v>16</v>
+      </c>
+      <c r="D53" s="11">
+        <v>17</v>
+      </c>
+      <c r="E53" s="11">
+        <v>18</v>
+      </c>
+      <c r="F53" s="11">
+        <v>19</v>
+      </c>
+      <c r="G53" s="11">
+        <v>20</v>
+      </c>
+      <c r="H53" s="11">
+        <v>21</v>
+      </c>
+      <c r="I53" s="11">
+        <v>22</v>
+      </c>
+      <c r="J53" s="11">
+        <v>23</v>
+      </c>
+      <c r="K53" s="11">
+        <v>24</v>
+      </c>
+      <c r="L53" s="2">
+        <v>25</v>
+      </c>
+      <c r="M53" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B54" s="1">
+        <v>3</v>
+      </c>
+      <c r="C54" s="1">
+        <v>3</v>
+      </c>
+      <c r="D54" s="1">
+        <v>3</v>
+      </c>
+      <c r="E54" s="1">
+        <v>3</v>
+      </c>
+      <c r="F54" s="1">
+        <v>3</v>
+      </c>
+      <c r="G54" s="1">
+        <v>3</v>
+      </c>
+      <c r="H54" s="1">
+        <v>3</v>
+      </c>
+      <c r="I54" s="1">
+        <v>3</v>
+      </c>
+      <c r="J54" s="1">
+        <v>3</v>
+      </c>
+      <c r="K54" s="1">
+        <v>3</v>
+      </c>
+      <c r="L54" s="1">
+        <v>3</v>
+      </c>
+      <c r="M54" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="L53" s="10"/>
-      <c r="M53" s="7"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B54" s="11">
-        <v>15</v>
-      </c>
-      <c r="C54" s="11">
-        <v>16</v>
-      </c>
-      <c r="D54" s="11">
-        <v>17</v>
-      </c>
-      <c r="E54" s="11">
-        <v>18</v>
-      </c>
-      <c r="F54" s="11">
-        <v>19</v>
-      </c>
-      <c r="G54" s="11">
-        <v>20</v>
-      </c>
-      <c r="H54" s="11">
-        <v>21</v>
-      </c>
-      <c r="I54" s="11">
-        <v>22</v>
-      </c>
-      <c r="J54" s="11">
-        <v>23</v>
-      </c>
-      <c r="K54" s="11">
-        <v>24</v>
-      </c>
-      <c r="L54" s="2">
-        <v>25</v>
-      </c>
-      <c r="M54" s="2">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B55" s="1">
-        <v>3</v>
-      </c>
-      <c r="C55" s="1">
-        <v>3</v>
-      </c>
-      <c r="D55" s="1">
-        <v>3</v>
-      </c>
-      <c r="E55" s="1">
-        <v>3</v>
-      </c>
-      <c r="F55" s="1">
-        <v>3</v>
-      </c>
-      <c r="G55" s="1">
-        <v>3</v>
-      </c>
-      <c r="H55" s="1">
-        <v>3</v>
-      </c>
-      <c r="I55" s="1">
-        <v>3</v>
-      </c>
-      <c r="J55" s="1">
-        <v>3</v>
-      </c>
-      <c r="K55" s="1">
-        <v>3</v>
-      </c>
-      <c r="L55" s="1">
-        <v>3</v>
-      </c>
-      <c r="M55" s="1">
-        <v>3</v>
+      <c r="C55" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B56" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J56" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="L56" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M56" s="1" t="s">
-        <v>95</v>
+      <c r="B56" s="13" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B57" s="13" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -1966,53 +2008,53 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B59" s="13" t="s">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>97</v>
       </c>
+      <c r="B60" s="2">
+        <v>0</v>
+      </c>
+      <c r="C60" s="2">
+        <v>1</v>
+      </c>
+      <c r="D60" s="2">
+        <v>2</v>
+      </c>
+      <c r="E60" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="B61" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B61" s="2">
-        <v>0</v>
-      </c>
-      <c r="C61" s="2">
-        <v>1</v>
-      </c>
-      <c r="D61" s="2">
-        <v>2</v>
-      </c>
-      <c r="E61" s="2">
-        <v>3</v>
+      <c r="C61" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B63" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E63" s="1" t="s">
+      <c r="B63" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2021,122 +2063,153 @@
         <v>107</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B67" s="2">
+        <v>0</v>
+      </c>
+      <c r="C67" s="2">
+        <v>1</v>
+      </c>
+      <c r="D67" s="2">
+        <v>2</v>
+      </c>
+      <c r="E67" s="2">
+        <v>3</v>
+      </c>
+      <c r="F67" s="2">
+        <v>4</v>
+      </c>
+      <c r="G67" s="2">
+        <v>5</v>
+      </c>
+      <c r="H67" s="2">
+        <v>6</v>
+      </c>
+      <c r="I67" s="2">
+        <v>7</v>
+      </c>
+      <c r="J67" s="2">
+        <v>8</v>
+      </c>
+      <c r="K67" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>110</v>
       </c>
-      <c r="B68" s="2">
-        <v>0</v>
-      </c>
-      <c r="C68" s="2">
+      <c r="B68" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D68" s="2">
-        <v>2</v>
-      </c>
-      <c r="E68" s="2">
-        <v>3</v>
-      </c>
-      <c r="F68" s="2">
-        <v>4</v>
-      </c>
-      <c r="G68" s="2">
-        <v>5</v>
-      </c>
-      <c r="H68" s="2">
+      <c r="E68" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F68" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I68" s="2">
-        <v>7</v>
-      </c>
-      <c r="J68" s="2">
-        <v>8</v>
-      </c>
-      <c r="K68" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G68" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>103</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="C69" s="1" t="s">
-        <v>4</v>
+        <v>112</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>20</v>
+        <v>114</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>25</v>
+        <v>117</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>26</v>
+        <v>113</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>104</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I70" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J70" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="K70" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B70" s="1">
+        <v>0</v>
+      </c>
+      <c r="C70" s="1">
+        <v>3</v>
+      </c>
+      <c r="D70" s="1">
+        <v>2</v>
+      </c>
+      <c r="E70" s="1">
+        <v>2</v>
+      </c>
+      <c r="F70" s="1">
+        <v>5</v>
+      </c>
+      <c r="G70" s="1">
+        <v>1</v>
+      </c>
+      <c r="H70" s="1">
+        <v>4</v>
+      </c>
+      <c r="I70" s="1">
+        <v>5</v>
+      </c>
+      <c r="J70" s="1">
+        <v>4</v>
+      </c>
+      <c r="K70" s="1">
+        <v>6</v>
+      </c>
+      <c r="O70" s="14"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>105</v>
       </c>
@@ -2144,81 +2217,154 @@
         <v>0</v>
       </c>
       <c r="C71" s="1">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D71" s="1">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E71" s="1">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F71" s="1">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G71" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="H71" s="1">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="I71" s="1">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="J71" s="1">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="K71" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>106</v>
-      </c>
-      <c r="B72" s="1">
         <v>0</v>
       </c>
-      <c r="C72" s="1">
-        <v>14</v>
-      </c>
-      <c r="D72" s="1">
-        <v>13</v>
-      </c>
-      <c r="E72" s="1">
-        <v>15</v>
-      </c>
-      <c r="F72" s="1">
-        <v>12</v>
-      </c>
-      <c r="G72" s="1">
-        <v>15</v>
-      </c>
-      <c r="H72" s="1">
-        <v>13</v>
-      </c>
-      <c r="I72" s="1">
-        <v>11</v>
-      </c>
-      <c r="J72" s="1">
-        <v>14</v>
-      </c>
-      <c r="K72" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B72" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B73" s="13" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B74" s="13" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B75" s="13" t="s">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>123</v>
+      </c>
+      <c r="B76" s="2">
+        <v>0</v>
+      </c>
+      <c r="C76" s="2">
+        <v>1</v>
+      </c>
+      <c r="D76" s="2">
+        <v>2</v>
+      </c>
+      <c r="E76" s="2">
+        <v>3</v>
+      </c>
+      <c r="F76" s="2">
+        <v>4</v>
+      </c>
+      <c r="G76" s="2">
+        <v>5</v>
+      </c>
+      <c r="H76" s="2">
+        <v>6</v>
+      </c>
+      <c r="I76" s="2">
+        <v>7</v>
+      </c>
+      <c r="J76" s="2">
+        <v>8</v>
+      </c>
+      <c r="K76" s="2">
+        <v>9</v>
+      </c>
+      <c r="L76" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B77" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L77" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B78" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C78" s="1">
+        <v>0</v>
+      </c>
+      <c r="D78" s="1">
+        <v>0</v>
+      </c>
+      <c r="E78" s="1">
+        <v>0</v>
+      </c>
+      <c r="F78" s="1">
+        <v>0</v>
+      </c>
+      <c r="G78" s="1">
+        <v>0</v>
+      </c>
+      <c r="H78" s="1">
+        <v>0</v>
+      </c>
+      <c r="I78" s="1">
+        <v>0</v>
+      </c>
+      <c r="J78" s="1">
+        <v>0</v>
+      </c>
+      <c r="K78" s="1">
+        <v>0</v>
+      </c>
+      <c r="L78" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>